<commit_message>
Use BTO data Income Tax regulations
</commit_message>
<xml_diff>
--- a/data-raw/beneficiary-tax-offset-by-fy.xlsx
+++ b/data-raw/beneficiary-tax-offset-by-fy.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughp\Documents\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26100" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26100" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>lowest_marginal_rate</t>
   </si>
@@ -93,13 +93,29 @@
   </si>
   <si>
     <t>1996-97</t>
+  </si>
+  <si>
+    <t>2014-15</t>
+  </si>
+  <si>
+    <t>2015-16</t>
+  </si>
+  <si>
+    <t>2016-17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,341 +460,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>37000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>37000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>37000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0.19</v>
-      </c>
-      <c r="C2">
-        <v>18200</v>
-      </c>
-      <c r="D2">
+      <c r="B5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D5" s="1">
         <v>37000</v>
       </c>
-      <c r="E2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E5" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>0.19</v>
-      </c>
-      <c r="C3">
-        <v>18200</v>
-      </c>
-      <c r="D3">
+      <c r="B6" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D6" s="1">
         <v>37000</v>
       </c>
-      <c r="E3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E6" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>0.15</v>
-      </c>
-      <c r="C4">
-        <v>6000</v>
-      </c>
-      <c r="D4">
+      <c r="B7" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D7" s="1">
         <v>35000</v>
       </c>
-      <c r="E4">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E7" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>0.15</v>
-      </c>
-      <c r="C5">
-        <v>6000</v>
-      </c>
-      <c r="D5">
+      <c r="B8" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D8" s="1">
         <v>35000</v>
       </c>
-      <c r="E5">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E8" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0.15</v>
-      </c>
-      <c r="C6">
-        <v>6000</v>
-      </c>
-      <c r="D6">
+      <c r="B9" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D9" s="1">
         <v>35000</v>
       </c>
-      <c r="E6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E9" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0.15</v>
-      </c>
-      <c r="C7">
-        <v>6000</v>
-      </c>
-      <c r="D7">
+      <c r="B10" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D10" s="1">
         <v>34000</v>
       </c>
-      <c r="E7">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E10" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>0.15</v>
-      </c>
-      <c r="C8">
-        <v>6000</v>
-      </c>
-      <c r="D8">
+      <c r="B11" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D11" s="1">
         <v>30000</v>
       </c>
-      <c r="E8">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E11" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>0.15</v>
-      </c>
-      <c r="C9">
-        <v>6000</v>
-      </c>
-      <c r="D9">
+      <c r="B12" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D12" s="1">
         <v>25000</v>
       </c>
-      <c r="E9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E12" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>0.15</v>
-      </c>
-      <c r="C10">
-        <v>6000</v>
-      </c>
-      <c r="D10">
+      <c r="B13" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D13" s="1">
         <v>21600</v>
       </c>
-      <c r="E10">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E13" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B14" s="1">
         <v>0.17</v>
       </c>
-      <c r="C11">
-        <v>6000</v>
-      </c>
-      <c r="D11">
+      <c r="C14" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D14" s="1">
         <v>21600</v>
       </c>
-      <c r="E11">
+      <c r="E14" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B15" s="1">
         <v>0.17</v>
       </c>
-      <c r="C12">
-        <v>6000</v>
-      </c>
-      <c r="D12">
+      <c r="C15" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D15" s="1">
         <v>21600</v>
       </c>
-      <c r="E12">
+      <c r="E15" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B16" s="1">
         <v>0.17</v>
       </c>
-      <c r="C13">
-        <v>6000</v>
-      </c>
-      <c r="D13">
+      <c r="C16" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D16" s="1">
         <v>20000</v>
       </c>
-      <c r="E13">
+      <c r="E16" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B17" s="1">
         <v>0.17</v>
       </c>
-      <c r="C14">
-        <v>6000</v>
-      </c>
-      <c r="D14">
+      <c r="C17" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D17" s="1">
         <v>20000</v>
       </c>
-      <c r="E14">
+      <c r="E17" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B18" s="1">
         <v>0.17</v>
       </c>
-      <c r="C15">
-        <v>6000</v>
-      </c>
-      <c r="D15">
+      <c r="C18" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D18" s="1">
         <v>20000</v>
       </c>
-      <c r="E15">
+      <c r="E18" s="1">
         <v>0.13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
+      <c r="B19" s="1">
         <v>0.2</v>
       </c>
-      <c r="C16">
+      <c r="C19" s="1">
         <v>5400</v>
       </c>
-      <c r="D16">
+      <c r="D19" s="1">
         <v>20700</v>
       </c>
-      <c r="E16">
+      <c r="E19" s="1">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
+      <c r="B20" s="1">
         <v>0.2</v>
       </c>
-      <c r="C17">
+      <c r="C20" s="1">
         <v>5400</v>
       </c>
-      <c r="D17">
+      <c r="D20" s="1">
         <v>20700</v>
       </c>
-      <c r="E17">
+      <c r="E20" s="1">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
+      <c r="B21" s="1">
         <v>0.2</v>
       </c>
-      <c r="C18">
+      <c r="C21" s="1">
         <v>5400</v>
       </c>
-      <c r="D18">
+      <c r="D21" s="1">
         <v>20700</v>
       </c>
-      <c r="E18">
+      <c r="E21" s="1">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
+      <c r="B22" s="1">
         <v>0.2</v>
       </c>
-      <c r="C19">
+      <c r="C22" s="1">
         <v>5400</v>
       </c>
-      <c r="D19">
+      <c r="D22" s="1">
         <v>20700</v>
       </c>
-      <c r="E19">
+      <c r="E22" s="1">
         <v>0.14000000000000001</v>
       </c>
     </row>

</xml_diff>